<commit_message>
IP warmup template file updated
</commit_message>
<xml_diff>
--- a/help/using/configuration/assets/IPWarmupPlan-Template.xlsx
+++ b/help/using/configuration/assets/IPWarmupPlan-Template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivamgoel/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliettemassardier/GitHub/journey-optimizer.en/journey-optimizer.en/help/using/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFCED35-0983-6245-9D55-BE3CAF50B921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{475492FE-DB6B-DE4A-8900-374501C56E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16500" xr2:uid="{9226B62C-221E-DA40-86E4-3FCD9A6CD7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Warmup Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Custom Domain Group" sheetId="3" r:id="rId2"/>
+    <sheet name="OOTB Domain Groups" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="283">
   <si>
     <t>Phase</t>
   </si>
@@ -73,6 +74,819 @@
   </si>
   <si>
     <t>Engagement Days</t>
+  </si>
+  <si>
+    <t>blu.it</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>gmail.com</t>
+  </si>
+  <si>
+    <t>googlemail.com</t>
+  </si>
+  <si>
+    <t>googlemail.co.uk</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>live.com</t>
+  </si>
+  <si>
+    <t>msn.com</t>
+  </si>
+  <si>
+    <t>hotmail.ca</t>
+  </si>
+  <si>
+    <t>hotmail.com</t>
+  </si>
+  <si>
+    <t>hotmail.de</t>
+  </si>
+  <si>
+    <t>hotmail.dk</t>
+  </si>
+  <si>
+    <t>hotmail.co.jp</t>
+  </si>
+  <si>
+    <t>hotmail.it</t>
+  </si>
+  <si>
+    <t>hotmail.es</t>
+  </si>
+  <si>
+    <t>hotmail.fr</t>
+  </si>
+  <si>
+    <t>hotmail.co.uk</t>
+  </si>
+  <si>
+    <t>hotmail.co.kr</t>
+  </si>
+  <si>
+    <t>hotmail.com.au</t>
+  </si>
+  <si>
+    <t>hotmail.com.ar</t>
+  </si>
+  <si>
+    <t>hotmail.co.il</t>
+  </si>
+  <si>
+    <t>hotmail.com.br</t>
+  </si>
+  <si>
+    <t>hotmail.com.tr</t>
+  </si>
+  <si>
+    <t>hotmail.co.th</t>
+  </si>
+  <si>
+    <t>hotmail.jp</t>
+  </si>
+  <si>
+    <t>hotmail.se</t>
+  </si>
+  <si>
+    <t>live.at</t>
+  </si>
+  <si>
+    <t>live.be</t>
+  </si>
+  <si>
+    <t>live.ca</t>
+  </si>
+  <si>
+    <t>live.cl</t>
+  </si>
+  <si>
+    <t>live.cn</t>
+  </si>
+  <si>
+    <t>live.co.kr</t>
+  </si>
+  <si>
+    <t>live.co.uk</t>
+  </si>
+  <si>
+    <t>live.com.ar</t>
+  </si>
+  <si>
+    <t>live.com.au</t>
+  </si>
+  <si>
+    <t>live.com.mx</t>
+  </si>
+  <si>
+    <t>live.com.my</t>
+  </si>
+  <si>
+    <t>live.com.sg</t>
+  </si>
+  <si>
+    <t>live.de</t>
+  </si>
+  <si>
+    <t>live.dk</t>
+  </si>
+  <si>
+    <t>live.fr</t>
+  </si>
+  <si>
+    <t>live.hk</t>
+  </si>
+  <si>
+    <t>live.ie</t>
+  </si>
+  <si>
+    <t>live.in</t>
+  </si>
+  <si>
+    <t>live.it</t>
+  </si>
+  <si>
+    <t>live.jp</t>
+  </si>
+  <si>
+    <t>live.nl</t>
+  </si>
+  <si>
+    <t>live.no</t>
+  </si>
+  <si>
+    <t>live.ru</t>
+  </si>
+  <si>
+    <t>live.se</t>
+  </si>
+  <si>
+    <t>outlook.com</t>
+  </si>
+  <si>
+    <t>hotmail.gr</t>
+  </si>
+  <si>
+    <t>windowslive.com</t>
+  </si>
+  <si>
+    <t>xbox.com</t>
+  </si>
+  <si>
+    <t>hotmail.cl</t>
+  </si>
+  <si>
+    <t>hotmail.ch</t>
+  </si>
+  <si>
+    <t>outlook.ie</t>
+  </si>
+  <si>
+    <t>outlook.com.br</t>
+  </si>
+  <si>
+    <t>live.com.pt</t>
+  </si>
+  <si>
+    <t>live.co.za</t>
+  </si>
+  <si>
+    <t>mts.net</t>
+  </si>
+  <si>
+    <t>Yahoo</t>
+  </si>
+  <si>
+    <t>yahoo.com</t>
+  </si>
+  <si>
+    <t>rocketmail.com</t>
+  </si>
+  <si>
+    <t>rogers.com</t>
+  </si>
+  <si>
+    <t>sky.com</t>
+  </si>
+  <si>
+    <t>talk21.com</t>
+  </si>
+  <si>
+    <t>y7mail.com</t>
+  </si>
+  <si>
+    <t>yahoo.at</t>
+  </si>
+  <si>
+    <t>yahoo.be</t>
+  </si>
+  <si>
+    <t>yahoo.bg</t>
+  </si>
+  <si>
+    <t>yahoo.ca</t>
+  </si>
+  <si>
+    <t>yahoo.cl</t>
+  </si>
+  <si>
+    <t>yahoo.co.hu</t>
+  </si>
+  <si>
+    <t>yahoo.co.id</t>
+  </si>
+  <si>
+    <t>yahoo.co.il</t>
+  </si>
+  <si>
+    <t>yahoo.co.in</t>
+  </si>
+  <si>
+    <t>yahoo.co.jp</t>
+  </si>
+  <si>
+    <t>yahoo.co.kr</t>
+  </si>
+  <si>
+    <t>yahoo.com.ar</t>
+  </si>
+  <si>
+    <t>yahoo.com.au</t>
+  </si>
+  <si>
+    <t>yahoo.com.biz</t>
+  </si>
+  <si>
+    <t>yahoo.com.br</t>
+  </si>
+  <si>
+    <t>yahoo.com.cn</t>
+  </si>
+  <si>
+    <t>yahoo.com.co</t>
+  </si>
+  <si>
+    <t>yahoo.com.hk</t>
+  </si>
+  <si>
+    <t>yahoo.com.hr</t>
+  </si>
+  <si>
+    <t>yahoo.com.in</t>
+  </si>
+  <si>
+    <t>yahoo.com.jp</t>
+  </si>
+  <si>
+    <t>yahoo.com.kr</t>
+  </si>
+  <si>
+    <t>yahoo.com.mx</t>
+  </si>
+  <si>
+    <t>yahoo.com.my</t>
+  </si>
+  <si>
+    <t>yahoo.com.net</t>
+  </si>
+  <si>
+    <t>yahoo.com.pe</t>
+  </si>
+  <si>
+    <t>yahoo.com.ph</t>
+  </si>
+  <si>
+    <t>yahoo.com.sg</t>
+  </si>
+  <si>
+    <t>yahoo.com.tr</t>
+  </si>
+  <si>
+    <t>yahoo.com.tw</t>
+  </si>
+  <si>
+    <t>yahoo.com.ua</t>
+  </si>
+  <si>
+    <t>yahoo.com.ve</t>
+  </si>
+  <si>
+    <t>yahoo.com.vn</t>
+  </si>
+  <si>
+    <t>yahoo.co.nz</t>
+  </si>
+  <si>
+    <t>yahoo.co.th</t>
+  </si>
+  <si>
+    <t>yahoo.co.uk</t>
+  </si>
+  <si>
+    <t>yahoo.co.za</t>
+  </si>
+  <si>
+    <t>yahoo.cz</t>
+  </si>
+  <si>
+    <t>yahoo.de</t>
+  </si>
+  <si>
+    <t>yahoo.dk</t>
+  </si>
+  <si>
+    <t>yahoo.ee</t>
+  </si>
+  <si>
+    <t>yahoo.es</t>
+  </si>
+  <si>
+    <t>yahoo.fi</t>
+  </si>
+  <si>
+    <t>yahoo.fr</t>
+  </si>
+  <si>
+    <t>yahoogroups.co.kr</t>
+  </si>
+  <si>
+    <t>yahoogroups.com.cn</t>
+  </si>
+  <si>
+    <t>yahoogroups.com.sg</t>
+  </si>
+  <si>
+    <t>yahoogroups.com.tw</t>
+  </si>
+  <si>
+    <t>yahoogrupper.dk</t>
+  </si>
+  <si>
+    <t>yahoogruppi.it</t>
+  </si>
+  <si>
+    <t>yahoo.gr</t>
+  </si>
+  <si>
+    <t>yahoo.hr</t>
+  </si>
+  <si>
+    <t>yahoo.hu</t>
+  </si>
+  <si>
+    <t>yahoo.ie</t>
+  </si>
+  <si>
+    <t>yahoo.in</t>
+  </si>
+  <si>
+    <t>yahoo.it</t>
+  </si>
+  <si>
+    <t>yahoo.lt</t>
+  </si>
+  <si>
+    <t>yahoo.lv</t>
+  </si>
+  <si>
+    <t>yahoo.nl</t>
+  </si>
+  <si>
+    <t>yahoo.no</t>
+  </si>
+  <si>
+    <t>yahoo.pl</t>
+  </si>
+  <si>
+    <t>yahoo.pt</t>
+  </si>
+  <si>
+    <t>yahoo.ro</t>
+  </si>
+  <si>
+    <t>yahoo.rs</t>
+  </si>
+  <si>
+    <t>yahoo.se</t>
+  </si>
+  <si>
+    <t>yahoo.si</t>
+  </si>
+  <si>
+    <t>yahoo.sk</t>
+  </si>
+  <si>
+    <t>yahooxtra.co.nz</t>
+  </si>
+  <si>
+    <t>ymail.com</t>
+  </si>
+  <si>
+    <t>aol.com</t>
+  </si>
+  <si>
+    <t>aim.com</t>
+  </si>
+  <si>
+    <t>compuserve.com</t>
+  </si>
+  <si>
+    <t>cs.com</t>
+  </si>
+  <si>
+    <t>netscape.com</t>
+  </si>
+  <si>
+    <t>netscape.net</t>
+  </si>
+  <si>
+    <t>wmconnect.com</t>
+  </si>
+  <si>
+    <t>aol.co.uk</t>
+  </si>
+  <si>
+    <t>aol.in</t>
+  </si>
+  <si>
+    <t>aol.de</t>
+  </si>
+  <si>
+    <t>aol.fr</t>
+  </si>
+  <si>
+    <t>aol.nl</t>
+  </si>
+  <si>
+    <t>aol.pl</t>
+  </si>
+  <si>
+    <t>aol.jp</t>
+  </si>
+  <si>
+    <t>aol.es</t>
+  </si>
+  <si>
+    <t>aol.it</t>
+  </si>
+  <si>
+    <t>aol.com.ar</t>
+  </si>
+  <si>
+    <t>aol.fi</t>
+  </si>
+  <si>
+    <t>aol.cl</t>
+  </si>
+  <si>
+    <t>aol.com.co</t>
+  </si>
+  <si>
+    <t>aol.com.ve</t>
+  </si>
+  <si>
+    <t>aol.com.au</t>
+  </si>
+  <si>
+    <t>aol.at</t>
+  </si>
+  <si>
+    <t>aol.be</t>
+  </si>
+  <si>
+    <t>aol.com.br</t>
+  </si>
+  <si>
+    <t>aol.cz</t>
+  </si>
+  <si>
+    <t>aol.dk</t>
+  </si>
+  <si>
+    <t>myaol.jp</t>
+  </si>
+  <si>
+    <t>aolnorge.no</t>
+  </si>
+  <si>
+    <t>aolpolska.pl</t>
+  </si>
+  <si>
+    <t>aolpolcka.pl</t>
+  </si>
+  <si>
+    <t>aolpoland.pl</t>
+  </si>
+  <si>
+    <t>aol.ru</t>
+  </si>
+  <si>
+    <t>aol.kr</t>
+  </si>
+  <si>
+    <t>aol.se</t>
+  </si>
+  <si>
+    <t>aol.ch</t>
+  </si>
+  <si>
+    <t>aol.com.tr</t>
+  </si>
+  <si>
+    <t>aol.co.nz</t>
+  </si>
+  <si>
+    <t>aolchina.com</t>
+  </si>
+  <si>
+    <t>aol.hk</t>
+  </si>
+  <si>
+    <t>aol.tw</t>
+  </si>
+  <si>
+    <t>luckymail.com</t>
+  </si>
+  <si>
+    <t>verizon.net</t>
+  </si>
+  <si>
+    <t>aol.com.mx</t>
+  </si>
+  <si>
+    <t>bellatlantic.net</t>
+  </si>
+  <si>
+    <t>citlink.net</t>
+  </si>
+  <si>
+    <t>frontier.com</t>
+  </si>
+  <si>
+    <t>frontiernet.net</t>
+  </si>
+  <si>
+    <t>games.com</t>
+  </si>
+  <si>
+    <t>goowy.com</t>
+  </si>
+  <si>
+    <t>gte.net</t>
+  </si>
+  <si>
+    <t>love.com</t>
+  </si>
+  <si>
+    <t>verizon.net.in</t>
+  </si>
+  <si>
+    <t>wild4music.com</t>
+  </si>
+  <si>
+    <t>wow.com</t>
+  </si>
+  <si>
+    <t>yahoo.cn</t>
+  </si>
+  <si>
+    <t>yahoo.ne.jp</t>
+  </si>
+  <si>
+    <t>yahoogroups.ca</t>
+  </si>
+  <si>
+    <t>yahoogroups.co.in</t>
+  </si>
+  <si>
+    <t>yahoogroups.co.uk</t>
+  </si>
+  <si>
+    <t>yahoogroups.com</t>
+  </si>
+  <si>
+    <t>yahoogroups.com.au</t>
+  </si>
+  <si>
+    <t>yahoogroups.com.hk</t>
+  </si>
+  <si>
+    <t>yahoogroups.de</t>
+  </si>
+  <si>
+    <t>ybb.ne.jp</t>
+  </si>
+  <si>
+    <t>ygm.com</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>mac.com</t>
+  </si>
+  <si>
+    <t>icloud.com</t>
+  </si>
+  <si>
+    <t>apple.com</t>
+  </si>
+  <si>
+    <t>me.com</t>
+  </si>
+  <si>
+    <t>Comcast</t>
+  </si>
+  <si>
+    <t>comcast.net</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>orange.fr</t>
+  </si>
+  <si>
+    <t>orange.com</t>
+  </si>
+  <si>
+    <t>wanadoo.fr</t>
+  </si>
+  <si>
+    <t>francetelecom.com</t>
+  </si>
+  <si>
+    <t>voila.fr</t>
+  </si>
+  <si>
+    <t>voila.com</t>
+  </si>
+  <si>
+    <t>La Poste</t>
+  </si>
+  <si>
+    <t>laposte.net</t>
+  </si>
+  <si>
+    <t>Italia Online</t>
+  </si>
+  <si>
+    <t>libero.it</t>
+  </si>
+  <si>
+    <t>inwind.it</t>
+  </si>
+  <si>
+    <t>iol.it</t>
+  </si>
+  <si>
+    <t>giallo.it</t>
+  </si>
+  <si>
+    <t>virgilio.it</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>wp.pl</t>
+  </si>
+  <si>
+    <t>o2.pl</t>
+  </si>
+  <si>
+    <t>United Internet</t>
+  </si>
+  <si>
+    <t>web.de</t>
+  </si>
+  <si>
+    <t>gmx.de</t>
+  </si>
+  <si>
+    <t>gmx.ch</t>
+  </si>
+  <si>
+    <t>gmx.net</t>
+  </si>
+  <si>
+    <t>gmx.com</t>
+  </si>
+  <si>
+    <t>gmx.at</t>
+  </si>
+  <si>
+    <t>gmx.fr</t>
+  </si>
+  <si>
+    <t>mail.com</t>
+  </si>
+  <si>
+    <t>1and1.com</t>
+  </si>
+  <si>
+    <t>1und1.de</t>
+  </si>
+  <si>
+    <t>Bigpond</t>
+  </si>
+  <si>
+    <t>bigpond.com</t>
+  </si>
+  <si>
+    <t>bigpond.net.au</t>
+  </si>
+  <si>
+    <t>bigpond.com.au</t>
+  </si>
+  <si>
+    <t>telstra.com</t>
+  </si>
+  <si>
+    <t>bigpond.net</t>
+  </si>
+  <si>
+    <t>Docomo</t>
+  </si>
+  <si>
+    <t>docomo.ne.jp</t>
+  </si>
+  <si>
+    <t>Softbank</t>
+  </si>
+  <si>
+    <t>softbank.ne.jp</t>
+  </si>
+  <si>
+    <t>c.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>d.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>h.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>k.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>n.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>q.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>r.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>s.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>t.vodafone.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-c.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-d.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-h.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-k.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-n.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-q.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-r.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-s.ne.jp</t>
+  </si>
+  <si>
+    <t>jp-t.ne.jp</t>
+  </si>
+  <si>
+    <t>KDDI</t>
+  </si>
+  <si>
+    <t>au.com</t>
+  </si>
+  <si>
+    <t>ezweb.ne.jp</t>
+  </si>
+  <si>
+    <t>uqmobile.jp</t>
   </si>
 </sst>
 </file>
@@ -481,9 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BFB7C4-CB6E-0447-ABD1-AF094073AF14}">
   <dimension ref="A1:U421"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10154,4 +10966,887 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A4A896-04CD-8740-AB36-3FC0B149222D}">
+  <dimension ref="A1:EL14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" t="s">
+        <v>91</v>
+      </c>
+      <c r="T3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>129</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>132</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>136</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>137</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>138</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>139</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>140</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>141</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>142</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>148</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>149</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>150</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>151</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>152</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>153</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>154</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>155</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>156</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>157</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>158</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>159</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>160</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>161</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>162</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>164</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>165</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>166</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>167</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>168</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>169</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>170</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>171</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>172</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>176</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>177</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>178</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>179</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>180</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>181</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>182</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>183</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>184</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>185</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>189</v>
+      </c>
+      <c r="DN3" t="s">
+        <v>190</v>
+      </c>
+      <c r="DO3" t="s">
+        <v>191</v>
+      </c>
+      <c r="DP3" t="s">
+        <v>192</v>
+      </c>
+      <c r="DQ3" t="s">
+        <v>193</v>
+      </c>
+      <c r="DR3" t="s">
+        <v>194</v>
+      </c>
+      <c r="DS3" t="s">
+        <v>195</v>
+      </c>
+      <c r="DT3" t="s">
+        <v>196</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>197</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>198</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>199</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>200</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>201</v>
+      </c>
+      <c r="DZ3" t="s">
+        <v>202</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>203</v>
+      </c>
+      <c r="EB3" t="s">
+        <v>204</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>205</v>
+      </c>
+      <c r="ED3" t="s">
+        <v>206</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>207</v>
+      </c>
+      <c r="EF3" t="s">
+        <v>208</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>209</v>
+      </c>
+      <c r="EH3" t="s">
+        <v>210</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>211</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>212</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EL3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I10" t="s">
+        <v>248</v>
+      </c>
+      <c r="J10" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G13" t="s">
+        <v>265</v>
+      </c>
+      <c r="H13" t="s">
+        <v>266</v>
+      </c>
+      <c r="I13" t="s">
+        <v>267</v>
+      </c>
+      <c r="J13" t="s">
+        <v>268</v>
+      </c>
+      <c r="K13" t="s">
+        <v>269</v>
+      </c>
+      <c r="L13" t="s">
+        <v>270</v>
+      </c>
+      <c r="M13" t="s">
+        <v>271</v>
+      </c>
+      <c r="N13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O13" t="s">
+        <v>273</v>
+      </c>
+      <c r="P13" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>275</v>
+      </c>
+      <c r="R13" t="s">
+        <v>276</v>
+      </c>
+      <c r="S13" t="s">
+        <v>277</v>
+      </c>
+      <c r="T13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:142" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IP warmup updated template file
</commit_message>
<xml_diff>
--- a/help/using/configuration/assets/IPWarmupPlan-Template.xlsx
+++ b/help/using/configuration/assets/IPWarmupPlan-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliettemassardier/GitHub/journey-optimizer.en/journey-optimizer.en/help/using/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{475492FE-DB6B-DE4A-8900-374501C56E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20A9FBE4-D046-C34F-B29B-9D5B28F2E97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16500" xr2:uid="{9226B62C-221E-DA40-86E4-3FCD9A6CD7AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{9226B62C-221E-DA40-86E4-3FCD9A6CD7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Warmup Plan" sheetId="1" r:id="rId1"/>

</xml_diff>